<commit_message>
Introduce DED column Content DE Name
Remove legacy 010 version since it is no longer compatible with the sample spreadsheet.
</commit_message>
<xml_diff>
--- a/cliprt/resources/sample.xlsx
+++ b/cliprt/resources/sample.xlsx
@@ -1,48 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhodges/VisualStudioCodeProjects/cliprt/cliprt/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6783AC-28B5-3047-B01B-60D748A32948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E424AFD5-2890-E947-A437-D9736DAF17E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="740" windowWidth="31940" windowHeight="18320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10240" yWindow="0" windowWidth="23360" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Elements" sheetId="1" r:id="rId1"/>
+    <sheet name="DED" sheetId="1" r:id="rId1"/>
     <sheet name="First Visit" sheetId="2" r:id="rId2"/>
     <sheet name="Mail List" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="214">
-  <si>
-    <t>Data Element</t>
-  </si>
-  <si>
-    <t>For Facebook targeting and API</t>
-  </si>
-  <si>
-    <t>For internal use (Searching and contacting)</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="204">
   <si>
     <t>Dest WS</t>
-  </si>
-  <si>
-    <t>Dest Element</t>
-  </si>
-  <si>
-    <t>DE Format</t>
   </si>
   <si>
     <t>client id</t>
@@ -60,13 +53,7 @@
     <t>profile creation date</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>referral name</t>
-  </si>
-  <si>
-    <t>Necessary</t>
   </si>
   <si>
     <t>ims</t>
@@ -87,28 +74,16 @@
     <t>name</t>
   </si>
   <si>
-    <t>name, identifier</t>
-  </si>
-  <si>
     <t>client</t>
   </si>
   <si>
     <t>client name</t>
   </si>
   <si>
-    <t>will parse last word to last name and rest to first name</t>
-  </si>
-  <si>
     <t>first name</t>
   </si>
   <si>
-    <t>name,fragment=1</t>
-  </si>
-  <si>
     <t>last name</t>
-  </si>
-  <si>
-    <t>name,fragment=2</t>
   </si>
   <si>
     <t>nickname</t>
@@ -117,19 +92,7 @@
     <t>phone</t>
   </si>
   <si>
-    <t>home phone will map to phone</t>
-  </si>
-  <si>
-    <t>phone, identifier</t>
-  </si>
-  <si>
     <t>home phone</t>
-  </si>
-  <si>
-    <t>Necessary ("home," etc. not)</t>
-  </si>
-  <si>
-    <t>mapped</t>
   </si>
   <si>
     <t>mobile phone</t>
@@ -665,6 +628,24 @@
   <si>
     <t>Alba, Patricia</t>
   </si>
+  <si>
+    <t>Content DE Name</t>
+  </si>
+  <si>
+    <t>Content DE Type</t>
+  </si>
+  <si>
+    <t>Dest DE Format</t>
+  </si>
+  <si>
+    <t>Dest DE Name</t>
+  </si>
+  <si>
+    <t>fragment=1</t>
+  </si>
+  <si>
+    <t>fragment=2</t>
+  </si>
 </sst>
 </file>
 
@@ -1139,462 +1120,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="50.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
+    <col min="1" max="5" width="19" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="17" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="17" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="D1" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B12" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
+      <c r="B13" s="1" t="s">
+        <v>203</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
+      <c r="D13" t="s">
+        <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
+      <c r="D16" t="s">
+        <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>14</v>
+      <c r="E16" t="s">
+        <v>18</v>
       </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
-        <v>8</v>
+      <c r="D17" t="s">
+        <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
+      <c r="C18" t="s">
+        <v>10</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
       </c>
-      <c r="G18" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="16"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="16"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="16"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="16"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="16"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
-        <v>14</v>
+      <c r="C34" t="s">
+        <v>7</v>
       </c>
-      <c r="C19" t="s">
-        <v>14</v>
+      <c r="E34" t="s">
+        <v>31</v>
       </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B35" s="16"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>56</v>
-      </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
-      <c r="G36" t="s">
-        <v>47</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1603,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H3086"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1623,28 +1490,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1652,25 +1519,25 @@
         <v>100005800</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="C2" s="3">
         <v>43882</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1678,25 +1545,25 @@
         <v>100003575</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3">
         <v>43564</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1704,25 +1571,25 @@
         <v>100003465</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C4" s="3">
         <v>43547</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1730,25 +1597,25 @@
         <v>100005413</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C5" s="3">
         <v>44022</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1756,25 +1623,25 @@
         <v>100005723</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C6" s="3">
         <v>43871</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1782,25 +1649,25 @@
         <v>100004341</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C7" s="3">
         <v>43673</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1808,25 +1675,25 @@
         <v>100006004</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C8" s="3">
         <v>43962</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1834,25 +1701,25 @@
         <v>100003248</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C9" s="3">
         <v>43494</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1860,25 +1727,25 @@
         <v>100005827</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C10" s="3">
         <v>43887</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1886,25 +1753,25 @@
         <v>100005308</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C11" s="3">
         <v>43825</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1912,25 +1779,25 @@
         <v>100005308</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C12" s="3">
         <v>43825</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1938,25 +1805,25 @@
         <v>100004798</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C13" s="3">
         <v>43743</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1964,25 +1831,25 @@
         <v>100001921</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C14" s="3">
         <v>42993</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1990,25 +1857,25 @@
         <v>100005504</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C15" s="3">
         <v>43847</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2016,25 +1883,25 @@
         <v>100002751</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C16" s="3">
         <v>43295</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -2042,25 +1909,25 @@
         <v>100002820</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C17" s="3">
         <v>43329</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -2068,25 +1935,25 @@
         <v>100003460</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C18" s="3">
         <v>43546</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -2094,25 +1961,25 @@
         <v>100005411</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C19" s="3">
         <v>43837</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -2120,25 +1987,25 @@
         <v>100004058</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C20" s="3">
         <v>43634</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3086" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2175,342 +2042,342 @@
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C2" s="11">
         <v>100005800</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="C3" s="11">
         <v>100000058</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C4" s="11">
         <v>100005310</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C5" s="11">
         <v>100003575</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C6" s="11">
         <v>100001587</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C7" s="11">
         <v>100001586</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C8" s="11">
         <v>100000536</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C9" s="11">
         <v>100003465</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C10" s="11">
         <v>100005413</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C11" s="11">
         <v>100000467</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C12" s="11">
         <v>100000468</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C13" s="11">
         <v>100001293</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C14" s="11">
         <v>100005723</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C15" s="11">
         <v>100004341</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="E15" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
-        <v>175</v>
-      </c>
       <c r="B16" s="21" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C16" s="11">
         <v>100000414</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C17" s="11">
         <v>100002322</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C18" s="11">
         <v>100006004</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C19" s="11">
         <v>100003248</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C20" s="11">
         <v>100005827</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>